<commit_message>
Ready for new Digikey BOM
</commit_message>
<xml_diff>
--- a/BOMs/Plane_Project_Digikey_BOM_V1.xlsx
+++ b/BOMs/Plane_Project_Digikey_BOM_V1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Caltech\SeniorYear\PlaneProject\BOMs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Caltech\SeniorYear\PlaneProject\GitFiles\BOMs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Plane_Project_BOM_V1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -1478,8 +1478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="H49" sqref="H49"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Finished Kicad BOM V2
</commit_message>
<xml_diff>
--- a/BOMs/Plane_Project_Digikey_BOM_V1.xlsx
+++ b/BOMs/Plane_Project_Digikey_BOM_V1.xlsx
@@ -1478,8 +1478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>